<commit_message>
JDBC performance data collection
</commit_message>
<xml_diff>
--- a/plot/data process.xlsx
+++ b/plot/data process.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="700" yWindow="2340" windowWidth="25600" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="-25600" yWindow="0" windowWidth="25600" windowHeight="17600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="16">
   <si>
     <t>d1</t>
   </si>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t>ORM 0NF</t>
+  </si>
+  <si>
+    <t>JDBC 3NF</t>
+  </si>
+  <si>
+    <t>JDBC 0NF</t>
   </si>
 </sst>
 </file>
@@ -130,8 +136,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="87">
+  <cellStyleXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -224,7 +232,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="87">
+  <cellStyles count="89">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -268,6 +276,7 @@
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -311,6 +320,7 @@
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -642,8 +652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:XFD33"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1179,9 +1189,17 @@
         <v>29.583576568707855</v>
       </c>
     </row>
+    <row r="19" spans="1:13">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19">
+        <v>21</v>
+      </c>
+    </row>
     <row r="20" spans="1:13">
       <c r="A20" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>11</v>
@@ -1228,19 +1246,19 @@
         <v>292571</v>
       </c>
       <c r="C21" s="2">
-        <v>1215222</v>
+        <v>702016</v>
       </c>
       <c r="D21" s="2">
-        <v>35.479999999999997</v>
+        <v>59.06</v>
       </c>
       <c r="E21" s="2">
-        <v>18.920000000000002</v>
+        <v>22.5</v>
       </c>
       <c r="F21" s="2">
         <v>0</v>
       </c>
       <c r="G21" s="2">
-        <v>13.3</v>
+        <v>1392.35</v>
       </c>
       <c r="H21" s="1">
         <f>B21</f>
@@ -1248,15 +1266,15 @@
       </c>
       <c r="I21" s="1">
         <f>C21</f>
-        <v>1215222</v>
+        <v>702016</v>
       </c>
       <c r="J21" s="1">
         <f>D21</f>
-        <v>35.479999999999997</v>
+        <v>59.06</v>
       </c>
       <c r="K21" s="1">
         <f>E21</f>
-        <v>18.920000000000002</v>
+        <v>22.5</v>
       </c>
       <c r="L21" s="1">
         <f>F21</f>
@@ -1264,7 +1282,7 @@
       </c>
       <c r="M21" s="1">
         <f>G21</f>
-        <v>13.3</v>
+        <v>1392.35</v>
       </c>
     </row>
     <row r="22" spans="1:13">
@@ -1275,19 +1293,19 @@
         <v>442309</v>
       </c>
       <c r="C22" s="2">
-        <v>1803110</v>
+        <v>959162</v>
       </c>
       <c r="D22" s="2">
-        <v>30.74</v>
+        <v>56.86</v>
       </c>
       <c r="E22" s="2">
-        <v>21.06</v>
+        <v>23.68</v>
       </c>
       <c r="F22" s="2">
         <v>0</v>
       </c>
       <c r="G22" s="2">
-        <v>21.18</v>
+        <v>1417.82</v>
       </c>
       <c r="H22" s="1">
         <f>SUM(B21:B22)</f>
@@ -1295,15 +1313,15 @@
       </c>
       <c r="I22" s="1">
         <f>SUM(C21:C22)</f>
-        <v>3018332</v>
+        <v>1661178</v>
       </c>
       <c r="J22" s="1">
         <f>(D21*$C21 + D22*$C22)/$I22</f>
-        <v>32.648389229547973</v>
+        <v>57.789722883399612</v>
       </c>
       <c r="K22" s="1">
         <f>(E21*$C21 + E22*$C22)/$I22</f>
-        <v>20.198406550372855</v>
+        <v>23.181330453449299</v>
       </c>
       <c r="L22" s="1">
         <f>(F21*$C21 + F22*$C22)/$I22</f>
@@ -1311,7 +1329,7 @@
       </c>
       <c r="M22" s="1">
         <f>(G21*$C21 + G22*$C22)/$I22</f>
-        <v>18.007403559316867</v>
+        <v>1407.0563446180961</v>
       </c>
     </row>
     <row r="23" spans="1:13">
@@ -1322,19 +1340,19 @@
         <v>469906</v>
       </c>
       <c r="C23" s="2">
-        <v>1971001</v>
+        <v>1061299</v>
       </c>
       <c r="D23" s="2">
-        <v>30.06</v>
+        <v>52.71</v>
       </c>
       <c r="E23" s="2">
-        <v>25.1</v>
+        <v>24.54</v>
       </c>
       <c r="F23" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>0.02</v>
       </c>
       <c r="G23" s="2">
-        <v>59.51</v>
+        <v>1336.32</v>
       </c>
       <c r="H23" s="1">
         <f>SUM(B21:B23)</f>
@@ -1342,23 +1360,23 @@
       </c>
       <c r="I23" s="1">
         <f>SUM(C21:C23)</f>
-        <v>4989333</v>
+        <v>2722477</v>
       </c>
       <c r="J23" s="1">
         <f>(D21*$C21+D22*$C22 + D23*$C23)/$I23</f>
-        <v>31.625864222732773</v>
+        <v>55.80950236494192</v>
       </c>
       <c r="K23" s="1">
         <f>(E21*$C21+E22*$C22 + E23*$C23)/$I23</f>
-        <v>22.134746656517013</v>
+        <v>23.710978502297724</v>
       </c>
       <c r="L23" s="1">
         <f>(F21*$C21+F22*$C22 + F23*$C23)/$I23</f>
-        <v>2.7653008929249663E-2</v>
+        <v>7.7965690802897503E-3</v>
       </c>
       <c r="M23" s="1">
         <f>(G21*$C21+G22*$C22 + G23*$C23)/$I23</f>
-        <v>34.402713130191948</v>
+        <v>1379.4813047529876</v>
       </c>
     </row>
     <row r="24" spans="1:13">
@@ -1369,19 +1387,19 @@
         <v>465048</v>
       </c>
       <c r="C24" s="2">
-        <v>1916735</v>
+        <v>1094690</v>
       </c>
       <c r="D24" s="2">
-        <v>29.53</v>
+        <v>49.31</v>
       </c>
       <c r="E24" s="2">
-        <v>26.32</v>
+        <v>25.13</v>
       </c>
       <c r="F24" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>0.13</v>
       </c>
       <c r="G24" s="2">
-        <v>82.89</v>
+        <v>1292.45</v>
       </c>
       <c r="H24" s="1">
         <f>SUM(B21:B24)</f>
@@ -1389,23 +1407,23 @@
       </c>
       <c r="I24" s="1">
         <f>SUM(C21:C24)</f>
-        <v>6906068</v>
+        <v>3817167</v>
       </c>
       <c r="J24" s="1">
         <f>(D21*$C21 +D22*$C22+D23*$C23 + D24*$C24)/$I24</f>
-        <v>31.044170513525206</v>
+        <v>53.945570227867947</v>
       </c>
       <c r="K24" s="1">
         <f>(E21*$C21 +E22*$C22+E23*$C23 + E24*$C24)/$I24</f>
-        <v>23.296336951793695</v>
+        <v>24.117926546048416</v>
       </c>
       <c r="L24" s="1">
         <f>(F21*$C21 +F22*$C22+F23*$C23 + F24*$C24)/$I24</f>
-        <v>3.9406145436158467E-2</v>
+        <v>4.2842160167474996E-2</v>
       </c>
       <c r="M24" s="1">
         <f>(G21*$C21 +G22*$C22+G23*$C23 + G24*$C24)/$I24</f>
-        <v>47.860049460850952</v>
+        <v>1354.5224022475304</v>
       </c>
     </row>
     <row r="25" spans="1:13">
@@ -1416,19 +1434,19 @@
         <v>454965</v>
       </c>
       <c r="C25" s="2">
-        <v>1956321</v>
+        <v>1120446</v>
       </c>
       <c r="D25" s="2">
-        <v>29.05</v>
+        <v>48.91</v>
       </c>
       <c r="E25" s="2">
-        <v>27.21</v>
+        <v>25.73</v>
       </c>
       <c r="F25" s="2">
-        <v>0.64</v>
+        <v>0.63</v>
       </c>
       <c r="G25" s="2">
-        <v>105.86</v>
+        <v>1237.6300000000001</v>
       </c>
       <c r="H25" s="1">
         <f>SUM(B21:B25)</f>
@@ -1436,28 +1454,28 @@
       </c>
       <c r="I25" s="1">
         <f>SUM(C21:C25)</f>
-        <v>8862389</v>
+        <v>4937613</v>
       </c>
       <c r="J25" s="1">
         <f>(D21*$C21 +D22*$C22 +D23*$C23+D24*$C24 + D25*$C25)/$I25</f>
-        <v>30.603968932079148</v>
+        <v>52.802895717019538</v>
       </c>
       <c r="K25" s="1">
         <f>(E21*$C21 +E22*$C22 +E23*$C23+E24*$C24 + E25*$C25)/$I25</f>
-        <v>24.160255383734565</v>
+        <v>24.483739187336067</v>
       </c>
       <c r="L25" s="1">
         <f>(F21*$C21 +F22*$C22 +F23*$C23+F24*$C24 + F25*$C25)/$I25</f>
-        <v>0.17198375742703237</v>
+        <v>0.17608035704701847</v>
       </c>
       <c r="M25" s="1">
         <f>(G21*$C21 +G22*$C22 +G23*$C23+G24*$C24 + G25*$C25)/$I25</f>
-        <v>60.663202339685157</v>
+        <v>1327.9971106686569</v>
       </c>
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
@@ -1497,39 +1515,39 @@
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2">
-        <v>229614</v>
+        <v>312518</v>
       </c>
       <c r="D29" s="2">
-        <v>66.19</v>
+        <v>53.22</v>
       </c>
       <c r="E29" s="2">
-        <v>20.309999999999999</v>
+        <v>22.49</v>
       </c>
       <c r="F29" s="2">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="G29" s="2">
-        <v>17.29</v>
+        <v>1979.29</v>
       </c>
       <c r="I29" s="1">
         <f>C29</f>
-        <v>229614</v>
+        <v>312518</v>
       </c>
       <c r="J29" s="1">
         <f>D29</f>
-        <v>66.19</v>
+        <v>53.22</v>
       </c>
       <c r="K29" s="1">
         <f>E29</f>
-        <v>20.309999999999999</v>
+        <v>22.49</v>
       </c>
       <c r="L29" s="1">
         <f>F29</f>
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="M29" s="1">
         <f>G29</f>
-        <v>17.29</v>
+        <v>1979.29</v>
       </c>
     </row>
     <row r="30" spans="1:13">
@@ -1538,39 +1556,39 @@
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2">
-        <v>310048</v>
+        <v>471503</v>
       </c>
       <c r="D30" s="2">
-        <v>65.989999999999995</v>
+        <v>46.59</v>
       </c>
       <c r="E30" s="2">
-        <v>22.53</v>
+        <v>22.63</v>
       </c>
       <c r="F30" s="2">
-        <v>0.16</v>
+        <v>0.32</v>
       </c>
       <c r="G30" s="2">
-        <v>23.34</v>
+        <v>2069.19</v>
       </c>
       <c r="I30" s="1">
         <f>SUM(C29:C30)</f>
-        <v>539662</v>
+        <v>784021</v>
       </c>
       <c r="J30" s="1">
         <f>(D29*$C29 + D30*$C30)/$I30</f>
-        <v>66.075095485692898</v>
+        <v>49.232779134742572</v>
       </c>
       <c r="K30" s="1">
         <f>(E29*$C29 + E30*$C30)/$I30</f>
-        <v>21.58544010880885</v>
+        <v>22.574194709070291</v>
       </c>
       <c r="L30" s="1">
         <f>(F29*$C29 + F30*$C30)/$I30</f>
-        <v>0.10043316001497234</v>
+        <v>0.19244504930352629</v>
       </c>
       <c r="M30" s="1">
         <f>(G29*$C29 + G30*$C30)/$I30</f>
-        <v>20.765861557789872</v>
+        <v>2033.3550310387093</v>
       </c>
     </row>
     <row r="31" spans="1:13">
@@ -1579,39 +1597,39 @@
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2">
-        <v>342307</v>
+        <v>495433</v>
       </c>
       <c r="D31" s="2">
-        <v>63.93</v>
+        <v>43.41</v>
       </c>
       <c r="E31" s="2">
-        <v>24.56</v>
+        <v>22.21</v>
       </c>
       <c r="F31" s="2">
-        <v>0.15</v>
+        <v>0.02</v>
       </c>
       <c r="G31" s="2">
-        <v>38.119999999999997</v>
+        <v>2091.42</v>
       </c>
       <c r="I31" s="1">
         <f>SUM(C29:C31)</f>
-        <v>881969</v>
+        <v>1279454</v>
       </c>
       <c r="J31" s="1">
         <f>(D29*$C29+D30*$C30 + D31*$C31)/$I31</f>
-        <v>65.242547855990395</v>
+        <v>46.97806975475477</v>
       </c>
       <c r="K31" s="1">
         <f>(E29*$C29+E30*$C30 + E31*$C31)/$I31</f>
-        <v>22.739916822473354</v>
+        <v>22.433170430511762</v>
       </c>
       <c r="L31" s="1">
         <f>(F29*$C29+F30*$C30 + F31*$C31)/$I31</f>
-        <v>0.11967088412404517</v>
+        <v>0.12567049694635368</v>
       </c>
       <c r="M31" s="1">
         <f>(G29*$C29+G30*$C30 + G31*$C31)/$I31</f>
-        <v>27.501294512618923</v>
+        <v>2055.8390763950874</v>
       </c>
     </row>
     <row r="32" spans="1:13">
@@ -1620,39 +1638,39 @@
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2">
-        <v>327326</v>
+        <v>488661</v>
       </c>
       <c r="D32" s="2">
-        <v>62.7</v>
+        <v>42.98</v>
       </c>
       <c r="E32" s="2">
-        <v>25.05</v>
+        <v>22.23</v>
       </c>
       <c r="F32" s="2">
-        <v>1.87</v>
+        <v>0.01</v>
       </c>
       <c r="G32" s="2">
-        <v>42.5</v>
+        <v>2073.0100000000002</v>
       </c>
       <c r="I32" s="1">
         <f>SUM(C29:C32)</f>
-        <v>1209295</v>
+        <v>1768115</v>
       </c>
       <c r="J32" s="1">
         <f>(D29*$C29 +D30*$C30+D31*$C31 + D32*$C32)/$I32</f>
-        <v>64.554343555542687</v>
+        <v>45.873107258294851</v>
       </c>
       <c r="K32" s="1">
         <f>(E29*$C29 +E30*$C30+E31*$C31 + E32*$C32)/$I32</f>
-        <v>23.36519873149232</v>
+        <v>22.377019407674272</v>
       </c>
       <c r="L32" s="1">
         <f>(F29*$C29 +F30*$C30+F31*$C31 + F32*$C32)/$I32</f>
-        <v>0.59344132738496402</v>
+        <v>9.370218000525983E-2</v>
       </c>
       <c r="M32" s="1">
         <f>(G29*$C29 +G30*$C30+G31*$C31 + G32*$C32)/$I32</f>
-        <v>31.561070061482102</v>
+        <v>2060.5846730897028</v>
       </c>
     </row>
     <row r="33" spans="1:13">
@@ -1677,23 +1695,23 @@
       </c>
       <c r="I33" s="1">
         <f>SUM(C29:C33)</f>
-        <v>1537619</v>
+        <v>2096439</v>
       </c>
       <c r="J33" s="1">
         <f>(D29*$C29 +D30*$C30 +D31*$C31+D32*$C32 + D33*$C33)/$I33</f>
-        <v>64.158390140860647</v>
+        <v>48.508372454433449</v>
       </c>
       <c r="K33" s="1">
         <f>(E29*$C29 +E30*$C30 +E31*$C31+E32*$C32 + E33*$C33)/$I33</f>
-        <v>23.861607823524555</v>
+        <v>22.895866385809459</v>
       </c>
       <c r="L33" s="1">
         <f>(F29*$C29 +F30*$C30 +F31*$C31+F32*$C32 + F33*$C33)/$I33</f>
-        <v>3.8084312368668702</v>
+        <v>2.5299790883493389</v>
       </c>
       <c r="M33" s="1">
         <f>(G29*$C29 +G30*$C30 +G31*$C31+G32*$C32 + G33*$C33)/$I33</f>
-        <v>29.583576568707855</v>
+        <v>1741.3682413177773</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
logstach conf and test data
</commit_message>
<xml_diff>
--- a/plot/data process.xlsx
+++ b/plot/data process.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="17">
   <si>
     <t>d1</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>JDBC 0NF</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -136,8 +139,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="89">
+  <cellStyleXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -232,7 +251,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="89">
+  <cellStyles count="105">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -277,6 +296,14 @@
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -321,6 +348,14 @@
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -652,8 +687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="L39" sqref="L39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1541,9 +1576,8 @@
         <f>E29</f>
         <v>22.49</v>
       </c>
-      <c r="L29" s="1">
-        <f>F29</f>
-        <v>0</v>
+      <c r="L29" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="M29" s="1">
         <f>G29</f>
@@ -1679,39 +1713,39 @@
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2">
-        <v>328324</v>
+        <v>482683</v>
       </c>
       <c r="D33" s="2">
-        <v>62.7</v>
+        <v>42.74</v>
       </c>
       <c r="E33" s="2">
-        <v>25.69</v>
+        <v>22.51</v>
       </c>
       <c r="F33" s="2">
-        <v>15.65</v>
+        <v>19.149999999999999</v>
       </c>
       <c r="G33" s="2">
-        <v>22.3</v>
+        <v>2046</v>
       </c>
       <c r="I33" s="1">
         <f>SUM(C29:C33)</f>
-        <v>2096439</v>
+        <v>2250798</v>
       </c>
       <c r="J33" s="1">
         <f>(D29*$C29 +D30*$C30 +D31*$C31+D32*$C32 + D33*$C33)/$I33</f>
-        <v>48.508372454433449</v>
+        <v>45.201213285243725</v>
       </c>
       <c r="K33" s="1">
         <f>(E29*$C29 +E30*$C30 +E31*$C31+E32*$C32 + E33*$C33)/$I33</f>
-        <v>22.895866385809459</v>
+        <v>22.405537058412168</v>
       </c>
       <c r="L33" s="1">
         <f>(F29*$C29 +F30*$C30 +F31*$C31+F32*$C32 + F33*$C33)/$I33</f>
-        <v>2.5299790883493389</v>
+        <v>4.1803199043183792</v>
       </c>
       <c r="M33" s="1">
         <f>(G29*$C29 +G30*$C30 +G31*$C31+G32*$C32 + G33*$C33)/$I33</f>
-        <v>1741.3682413177773</v>
+        <v>2057.4569940350048</v>
       </c>
     </row>
   </sheetData>

</xml_diff>